<commit_message>
Included today's DU in Weekly DU File
</commit_message>
<xml_diff>
--- a/documents/G8T9 - Week 4 DU.xlsx
+++ b/documents/G8T9 - Week 4 DU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPM Project\project-g8t9\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415DF717-2124-462F-9DC6-CB37B76870F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3857518-B20D-4D40-93A8-5F38B8F21A0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="3675" windowWidth="25935" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 4 Fri" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Question</t>
   </si>
@@ -133,6 +133,39 @@
   </si>
   <si>
     <t>Set up automatic reminders for daily updates and bug metrics updates, schedule timings for everyone to follow, leran json, github &amp; bootstrap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Went through wiki to check for new requirement changes </t>
+  </si>
+  <si>
+    <t>Created sql table using the sql file created  done by Lifu and read through the codes uploaded by the team</t>
+  </si>
+  <si>
+    <t>NIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start coding the UI of the homepage </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Upload the login and its form processing page</t>
+  </si>
+  <si>
+    <t>Revising on what was taught last year (eg: php, html)</t>
+  </si>
+  <si>
+    <t>Coding of the mainpage, (eg: showing the credit balance, student name, and etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upload the DAOs and classes, meet up with christine for pair programming </t>
+  </si>
+  <si>
+    <t>go through and see what other functions are necessary for the DAOs</t>
+  </si>
+  <si>
+    <t>Revised Data Management materials from last sem, created SQL files for SPM</t>
+  </si>
+  <si>
+    <t>Read through teammates' codes, update project schedule file</t>
   </si>
 </sst>
 </file>
@@ -549,8 +582,8 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E4" sqref="E4"/>
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -657,7 +690,9 @@
       <c r="G3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="11"/>
+      <c r="H3" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -674,7 +709,9 @@
       <c r="G4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -691,7 +728,9 @@
       <c r="G5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -710,7 +749,9 @@
       <c r="G6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="11"/>
+      <c r="H6" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -727,7 +768,9 @@
       <c r="G7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -744,7 +787,9 @@
       <c r="G8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -763,7 +808,9 @@
       <c r="G9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -780,7 +827,9 @@
       <c r="G10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="11"/>
+      <c r="H10" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -797,7 +846,9 @@
       <c r="G11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -816,7 +867,9 @@
       <c r="G12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -833,7 +886,9 @@
       <c r="G13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -850,7 +905,9 @@
       <c r="G14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -869,7 +926,9 @@
       <c r="G15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="11"/>
+      <c r="H15" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -886,7 +945,9 @@
       <c r="G16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="11"/>
+      <c r="H16" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="I16" s="11"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -903,7 +964,9 @@
       <c r="G17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">

</xml_diff>